<commit_message>
updates with Power BI - First part finished and ´published
</commit_message>
<xml_diff>
--- a/Budget/Sent Over Data - SalesBudget.xlsx
+++ b/Budget/Sent Over Data - SalesBudget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28817"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PORTFOLIO\AdventureWorks_Portfolio\Budget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551D7D98-A972-492A-8C8F-D4B2E9A444A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5F8E2D-4752-444E-9E85-498D803F926C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="11385" xr2:uid="{5CABF058-C44E-4B4C-A322-6CA47C838A4D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{5CABF058-C44E-4B4C-A322-6CA47C838A4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="1" r:id="rId1"/>
@@ -102,11 +102,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -422,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D3E0CB-37F1-4778-A2AE-5F0FF4562B38}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,103 +445,105 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>45292</v>
-      </c>
-      <c r="B2" s="2">
-        <v>800000</v>
+        <v>44927</v>
+      </c>
+      <c r="B2" s="4">
+        <f>B14*0.5</f>
+        <v>400000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>45323</v>
-      </c>
-      <c r="B3" s="2">
-        <v>800000</v>
+        <v>44958</v>
+      </c>
+      <c r="B3" s="4">
+        <f t="shared" ref="B3:B13" si="0">B15*0.5</f>
+        <v>400000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>45352</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1000000</v>
+        <v>44986</v>
+      </c>
+      <c r="B4" s="4">
+        <v>400000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>45383</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1000000</v>
+        <v>45017</v>
+      </c>
+      <c r="B5" s="4">
+        <v>400000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>45413</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1100000</v>
+        <v>45047</v>
+      </c>
+      <c r="B6" s="4">
+        <v>500000</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>45444</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1100000</v>
+        <v>45078</v>
+      </c>
+      <c r="B7" s="4">
+        <v>500000</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>45474</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1500000</v>
+        <v>45108</v>
+      </c>
+      <c r="B8" s="4">
+        <v>500000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>45505</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1500000</v>
+        <v>45139</v>
+      </c>
+      <c r="B9" s="4">
+        <v>500000</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>45536</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1500000</v>
+        <v>45170</v>
+      </c>
+      <c r="B10" s="4">
+        <v>550000</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>45566</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1500000</v>
+        <v>45200</v>
+      </c>
+      <c r="B11" s="4">
+        <v>550000</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>45597</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1500000</v>
+        <v>45231</v>
+      </c>
+      <c r="B12" s="4">
+        <v>550000</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>45627</v>
-      </c>
-      <c r="B13" s="2">
-        <v>2000000</v>
+        <v>45261</v>
+      </c>
+      <c r="B13" s="4">
+        <v>550000</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>45658</v>
+        <v>45292</v>
       </c>
       <c r="B14" s="2">
         <v>800000</v>
@@ -548,7 +551,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>45689</v>
+        <v>45323</v>
       </c>
       <c r="B15" s="2">
         <v>800000</v>
@@ -556,7 +559,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>45717</v>
+        <v>45352</v>
       </c>
       <c r="B16" s="2">
         <v>1000000</v>
@@ -564,7 +567,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>45748</v>
+        <v>45383</v>
       </c>
       <c r="B17" s="2">
         <v>1000000</v>
@@ -572,7 +575,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>45778</v>
+        <v>45413</v>
       </c>
       <c r="B18" s="2">
         <v>1100000</v>
@@ -580,9 +583,105 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
+        <v>45444</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1100000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>45474</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>45505</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>45536</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>45566</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>45597</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>45627</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>45658</v>
+      </c>
+      <c r="B26" s="2">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>45689</v>
+      </c>
+      <c r="B27" s="2">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>45717</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>45748</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>45778</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1100000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
         <v>45809</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B31" s="2">
         <v>1100000</v>
       </c>
     </row>

</xml_diff>